<commit_message>
Update Tracker testing spreadsheet
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wochristian/J2SProjects/GitHubOSP/tracker/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DF78BFCB-EFE8-5F45-A5E6-69FAA3DD8DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{57025516-0A2E-9241-9B80-DE58D4A1684E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="1460" windowWidth="36660" windowHeight="19640"/>
+    <workbookView xWindow="4520" yWindow="7140" windowWidth="36660" windowHeight="19640"/>
   </bookViews>
   <sheets>
     <sheet name="ComPADRE_tracker_experiments" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
add columns to verify mp4 conversion and Tracker 5.1.5 compatibility
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wochristian/J2SProjects/GitHubOSP/tracker/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678095B1-9316-F84B-A28D-F442343B2BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEFD61E-3313-4453-BD14-44AA9A881993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38760" yWindow="1060" windowWidth="36660" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ComPADRE_tracker_experiments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
   <si>
     <t>Tracker/Excel/Python/Tracker Data Analysis  (fly fishing)</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Uniform Motion 2010, Aaron Titus</t>
   </si>
   <si>
-    <t>2-D Collision of Pucks -- Center of Mass Velocity, Aaron Titus, recently updated</t>
-  </si>
-  <si>
     <t>Fluorescence Spectra, DB</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>The Motion Of A Spring Released From Uniform Circular Motion (2 TRZ files)</t>
   </si>
   <si>
-    <t>T. Online</t>
-  </si>
-  <si>
     <t>Sync OK?</t>
   </si>
   <si>
@@ -236,6 +230,18 @@
   </si>
   <si>
     <t>Spectra experiment page did not save correctly when TRZ was created.  Maybe convert experiment page to PDF?</t>
+  </si>
+  <si>
+    <t>ver5 OK?</t>
+  </si>
+  <si>
+    <t>2-D Collision of Pucks -- Center of Mass Velocity 2011, Aaron Titus</t>
+  </si>
+  <si>
+    <t>Online?</t>
+  </si>
+  <si>
+    <t>mp4?</t>
   </si>
 </sst>
 </file>
@@ -1083,663 +1089,681 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="70.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="7.296875" customWidth="1"/>
+    <col min="2" max="2" width="65.8984375" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" customWidth="1"/>
+    <col min="4" max="5" width="6.09765625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
       <c r="C37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="E48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
-      </c>
-      <c r="E54" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="G54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="G55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished testing all 59 TRZ files in JavaScript
4 files do not work properly.
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wochristian/J2SProjects/GitHubOSP/tracker/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEFD61E-3313-4453-BD14-44AA9A881993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8D4188-7B72-5C4D-8C2B-126AA51A9705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-42360" yWindow="620" windowWidth="38020" windowHeight="26960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ComPADRE_tracker_experiments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="75">
   <si>
     <t>Tracker/Excel/Python/Tracker Data Analysis  (fly fishing)</t>
   </si>
@@ -199,9 +199,6 @@
     <t>mp4</t>
   </si>
   <si>
-    <t>Will not convert to TRZ</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -242,13 +239,19 @@
   </si>
   <si>
     <t>mp4?</t>
+  </si>
+  <si>
+    <t>BH recommends users be asked if they wish to open Python code.</t>
+  </si>
+  <si>
+    <t>Cannot not convert zip to TRZ with mp4  video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,6 +386,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -687,7 +698,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -730,12 +741,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -769,6 +786,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1092,684 +1110,722 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.296875" customWidth="1"/>
-    <col min="2" max="2" width="65.8984375" customWidth="1"/>
-    <col min="3" max="3" width="8.59765625" customWidth="1"/>
-    <col min="4" max="5" width="6.09765625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
         <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
       </c>
       <c r="C27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
         <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
         <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
       <c r="B50" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>59</v>
+      </c>
       <c r="B53" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G54" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G55" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>50</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B61">
     <sortCondition ref="B2:B61"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{06FE2BF2-3799-6547-81CE-9E3024C27EE3}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{56F26E9B-74ED-0045-A6B9-3274F8D071E9}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{ABA14703-41A2-AA49-9EE5-52DD69194DB6}"/>
+    <hyperlink ref="B56" r:id="rId4" xr:uid="{5AE92896-7992-5146-B9DF-DE07212F5943}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed several issues, removed yellow highlights
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wochristian/J2SProjects/GitHubOSP/tracker/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8D4188-7B72-5C4D-8C2B-126AA51A9705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D601C49-7885-49D8-AD65-31B3A671E5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42360" yWindow="620" windowWidth="38020" windowHeight="26960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ComPADRE_tracker_experiments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="74">
   <si>
     <t>Tracker/Excel/Python/Tracker Data Analysis  (fly fishing)</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Diabolo Challenge at University of Oviedo</t>
   </si>
   <si>
-    <t xml:space="preserve">Damping of a Compass Video Analysis Activity </t>
-  </si>
-  <si>
     <t>Teaching Kinematics With Angry Birds</t>
   </si>
   <si>
@@ -214,21 +211,12 @@
     <t>JavaScript Notes</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>last frame appears at beginning of clip</t>
-  </si>
-  <si>
     <t>Using Tracker to understand ‚toss up‚ and free fall motion, Loo Kang</t>
   </si>
   <si>
-    <t>Spectra experiment page did not save correctly when TRZ was created.  Maybe convert experiment page to PDF?</t>
-  </si>
-  <si>
     <t>ver5 OK?</t>
   </si>
   <si>
@@ -238,13 +226,22 @@
     <t>Online?</t>
   </si>
   <si>
-    <t>mp4?</t>
-  </si>
-  <si>
     <t>BH recommends users be asked if they wish to open Python code.</t>
   </si>
   <si>
     <t>Cannot not convert zip to TRZ with mp4  video</t>
+  </si>
+  <si>
+    <t>mp4 or image?</t>
+  </si>
+  <si>
+    <t>Converted HTML instructions to PDF</t>
+  </si>
+  <si>
+    <t>Damping of a Compass Video Analysis Activity</t>
+  </si>
+  <si>
+    <t>trimmed videos to eliminate bad first frame</t>
   </si>
 </sst>
 </file>
@@ -743,14 +740,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1110,710 +1105,734 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="65.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.296875" customWidth="1"/>
+    <col min="2" max="2" width="65.796875" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" customWidth="1"/>
+    <col min="4" max="4" width="12.8984375" customWidth="1"/>
+    <col min="5" max="5" width="8.296875" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
       </c>
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" t="s">
-        <v>55</v>
-      </c>
       <c r="C37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
         <v>34</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G54" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
       </c>
       <c r="C55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1821,7 +1840,7 @@
     <sortCondition ref="B2:B61"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{06FE2BF2-3799-6547-81CE-9E3024C27EE3}"/>
+    <hyperlink ref="B8" r:id="rId1" display="Damping of a Compass Video Analysis Activity " xr:uid="{06FE2BF2-3799-6547-81CE-9E3024C27EE3}"/>
     <hyperlink ref="B17" r:id="rId2" xr:uid="{56F26E9B-74ED-0045-A6B9-3274F8D071E9}"/>
     <hyperlink ref="B28" r:id="rId3" xr:uid="{ABA14703-41A2-AA49-9EE5-52DD69194DB6}"/>
     <hyperlink ref="B56" r:id="rId4" xr:uid="{5AE92896-7992-5146-B9DF-DE07212F5943}"/>

</xml_diff>

<commit_message>
Replaced html support file with pdf in ComPASS trz.
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wochristian/J2SProjects/GitHubOSP/tracker/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D601C49-7885-49D8-AD65-31B3A671E5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE601349-40D0-FC43-9153-06BA8A817369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-41520" yWindow="2020" windowWidth="39740" windowHeight="24120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ComPADRE_tracker_experiments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="74">
   <si>
     <t>Tracker/Excel/Python/Tracker Data Analysis  (fly fishing)</t>
   </si>
@@ -202,9 +202,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>fails to load in Tracker Online</t>
-  </si>
-  <si>
     <t>Java Notes</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>trimmed videos to eliminate bad first frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orginal zip file had an html support file.  </t>
   </si>
 </sst>
 </file>
@@ -744,8 +744,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1105,48 +1105,48 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.296875" customWidth="1"/>
-    <col min="2" max="2" width="65.796875" customWidth="1"/>
-    <col min="3" max="3" width="8.69921875" customWidth="1"/>
-    <col min="4" max="4" width="12.8984375" customWidth="1"/>
-    <col min="5" max="5" width="8.296875" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
       <c r="C2" t="s">
         <v>58</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1224,18 +1224,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1290,7 +1293,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1323,27 +1326,27 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1373,10 +1376,10 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1384,10 +1387,10 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1395,10 +1398,10 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1428,10 +1431,10 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1450,30 +1453,30 @@
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1525,10 +1528,10 @@
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1536,10 +1539,10 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1682,7 +1685,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1726,10 +1729,10 @@
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1746,10 +1749,10 @@
         <v>58</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1788,7 +1791,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -1799,21 +1802,21 @@
         <v>59</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
updated with completed tests
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wochristian/J2SProjects/GitHubOSP/tracker/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE601349-40D0-FC43-9153-06BA8A817369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A077F17F-2A71-4565-A859-5E477EED95DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41520" yWindow="2020" windowWidth="39740" windowHeight="24120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ComPADRE_tracker_experiments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="74">
   <si>
     <t>Tracker/Excel/Python/Tracker Data Analysis  (fly fishing)</t>
   </si>
@@ -740,12 +740,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1105,22 +1104,22 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="65.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.296875" customWidth="1"/>
+    <col min="2" max="2" width="65.796875" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" customWidth="1"/>
+    <col min="4" max="4" width="12.796875" customWidth="1"/>
+    <col min="5" max="5" width="8.296875" customWidth="1"/>
+    <col min="6" max="6" width="11.296875" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1140,7 +1139,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1174,7 +1173,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1184,8 +1183,14 @@
       <c r="C4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1195,8 +1200,14 @@
       <c r="C5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1213,7 +1224,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1223,22 +1234,34 @@
       <c r="C7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1248,8 +1271,14 @@
       <c r="C9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1259,8 +1288,14 @@
       <c r="C10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1270,8 +1305,14 @@
       <c r="C11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1281,8 +1322,14 @@
       <c r="C12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1292,8 +1339,14 @@
       <c r="C13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1303,8 +1356,14 @@
       <c r="C14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1314,8 +1373,14 @@
       <c r="C15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1325,8 +1390,14 @@
       <c r="C16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1346,7 +1417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1356,8 +1427,14 @@
       <c r="C18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1367,8 +1444,14 @@
       <c r="C19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1378,8 +1461,14 @@
       <c r="C20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1389,8 +1478,14 @@
       <c r="C21" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1400,8 +1495,14 @@
       <c r="C22" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1411,8 +1512,14 @@
       <c r="C23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1422,8 +1529,14 @@
       <c r="C24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1433,8 +1546,14 @@
       <c r="C25" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1444,8 +1563,14 @@
       <c r="C26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1455,8 +1580,14 @@
       <c r="C27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1476,7 +1607,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1486,8 +1617,14 @@
       <c r="C29" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1497,8 +1634,14 @@
       <c r="C30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1508,8 +1651,14 @@
       <c r="C31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1519,8 +1668,14 @@
       <c r="C32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1530,8 +1685,14 @@
       <c r="C33" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1541,8 +1702,14 @@
       <c r="C34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -1552,8 +1719,14 @@
       <c r="C35" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -1563,8 +1736,14 @@
       <c r="C36" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -1574,8 +1753,14 @@
       <c r="C37" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -1585,8 +1770,14 @@
       <c r="C38" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -1597,7 +1788,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -1608,7 +1799,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -1619,7 +1810,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -1630,7 +1821,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -1641,7 +1832,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -1652,7 +1843,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1663,7 +1854,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -1674,7 +1865,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1685,7 +1876,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -1695,11 +1886,14 @@
       <c r="C48" t="s">
         <v>58</v>
       </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
       <c r="E48" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -1710,7 +1904,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1721,7 +1915,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1732,7 +1926,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1752,7 +1946,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -1763,7 +1957,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1777,7 +1971,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1791,7 +1985,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -1805,7 +1999,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1816,7 +2010,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1827,7 +2021,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
updated ComPADRE experiment list spreadsheet--nearly done
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A077F17F-2A71-4565-A859-5E477EED95DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F18EAF-050F-4956-9088-1211C456ECF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="77">
   <si>
     <t>Tracker/Excel/Python/Tracker Data Analysis  (fly fishing)</t>
   </si>
@@ -190,12 +190,6 @@
     <t>Sync OK?</t>
   </si>
   <si>
-    <t>image stack</t>
-  </si>
-  <si>
-    <t>mp4</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -226,9 +220,6 @@
     <t>BH recommends users be asked if they wish to open Python code.</t>
   </si>
   <si>
-    <t>Cannot not convert zip to TRZ with mp4  video</t>
-  </si>
-  <si>
     <t>mp4 or image?</t>
   </si>
   <si>
@@ -242,13 +233,31 @@
   </si>
   <si>
     <t xml:space="preserve">Orginal zip file had an html support file.  </t>
+  </si>
+  <si>
+    <t>corrected spelling of "crash"</t>
+  </si>
+  <si>
+    <t>v 6.0.9</t>
+  </si>
+  <si>
+    <t>no link</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>bad original flv video--freeze frame start</t>
+  </si>
+  <si>
+    <t>spreadsheet does not open with Tracker online</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,14 +392,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -695,7 +696,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -738,15 +739,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -780,7 +779,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1101,11 +1099,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:E10"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1121,927 +1119,1033 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>73</v>
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
         <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
         <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C42" t="s">
-        <v>58</v>
+      <c r="C42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" t="s">
+        <v>56</v>
+      </c>
+      <c r="E50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C51" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E52" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
         <v>34</v>
       </c>
       <c r="C53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" t="s">
-        <v>59</v>
-      </c>
-      <c r="G54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
-      </c>
-      <c r="G55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="D55" t="s">
+        <v>56</v>
+      </c>
+      <c r="E55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C57" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
-      <c r="C58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
         <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
+        <v>56</v>
+      </c>
+      <c r="E59" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B61">
     <sortCondition ref="B2:B61"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="Damping of a Compass Video Analysis Activity " xr:uid="{06FE2BF2-3799-6547-81CE-9E3024C27EE3}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{56F26E9B-74ED-0045-A6B9-3274F8D071E9}"/>
-    <hyperlink ref="B28" r:id="rId3" xr:uid="{ABA14703-41A2-AA49-9EE5-52DD69194DB6}"/>
-    <hyperlink ref="B56" r:id="rId4" xr:uid="{5AE92896-7992-5146-B9DF-DE07212F5943}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
updated ComPADRE experiment list
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F18EAF-050F-4956-9088-1211C456ECF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED5EB03-AE7F-47B6-8438-8DA249E2B3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="74">
   <si>
     <t>Tracker/Excel/Python/Tracker Data Analysis  (fly fishing)</t>
   </si>
@@ -193,9 +193,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Java Notes</t>
   </si>
   <si>
@@ -241,16 +238,10 @@
     <t>v 6.0.9</t>
   </si>
   <si>
-    <t>no link</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
     <t>bad original flv video--freeze frame start</t>
   </si>
   <si>
-    <t>spreadsheet does not open with Tracker online</t>
+    <t>works for Wolfgang</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1093,8 @@
   <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1119,22 +1110,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
         <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1142,7 +1133,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
@@ -1188,7 +1179,7 @@
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1246,8 +1237,8 @@
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>68</v>
+      <c r="B8" t="s">
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>56</v>
@@ -1259,7 +1250,7 @@
         <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1402,7 +1393,7 @@
       <c r="A17" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
       <c r="C17" t="s">
@@ -1415,7 +1406,7 @@
         <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1460,7 +1451,7 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
@@ -1477,7 +1468,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
@@ -1494,7 +1485,7 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
         <v>56</v>
@@ -1545,7 +1536,7 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
         <v>56</v>
@@ -1579,7 +1570,7 @@
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
         <v>56</v>
@@ -1592,7 +1583,7 @@
       <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>36</v>
       </c>
       <c r="C28" t="s">
@@ -1605,7 +1596,7 @@
         <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1684,7 +1675,7 @@
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
         <v>56</v>
@@ -1701,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
         <v>56</v>
@@ -1809,7 +1800,7 @@
         <v>56</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1826,24 +1817,24 @@
         <v>56</v>
       </c>
       <c r="E41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>72</v>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1860,7 +1851,7 @@
         <v>56</v>
       </c>
       <c r="E43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1983,14 +1974,14 @@
       </c>
     </row>
     <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>57</v>
+      <c r="A51" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>56</v>
@@ -1998,13 +1989,9 @@
       <c r="E51" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H51" s="1"/>
+      <c r="G51" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -2023,7 +2010,7 @@
         <v>56</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2045,24 +2032,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="2" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="C54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" t="s">
         <v>56</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G54" s="1"/>
     </row>
@@ -2083,20 +2070,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="2" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="C56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2105,7 +2092,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
         <v>56</v>
@@ -2123,6 +2110,15 @@
       </c>
       <c r="B58" t="s">
         <v>14</v>
+      </c>
+      <c r="C58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
all ComPADRE Tracker resources have now been tested/fixed :-)
</commit_message>
<xml_diff>
--- a/support/ComPADRE_tracker_experiments.xlsx
+++ b/support/ComPADRE_tracker_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobro\Eclipse\workspace_trackerJS\tracker\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED5EB03-AE7F-47B6-8438-8DA249E2B3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27AE2E-F77A-4F2E-9483-9438D8AE3807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>Tracker Video Analysis: Bouncing Ball Loo Kang, recenty updated</t>
   </si>
   <si>
-    <t>Two-Ball Collision Tracker Experiment 2019</t>
-  </si>
-  <si>
     <t>Tracker Video Modeling with Spreadsheets 2016</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>Online?</t>
   </si>
   <si>
-    <t>BH recommends users be asked if they wish to open Python code.</t>
-  </si>
-  <si>
     <t>mp4 or image?</t>
   </si>
   <si>
@@ -242,6 +236,12 @@
   </si>
   <si>
     <t>works for Wolfgang</t>
+  </si>
+  <si>
+    <t>Ask to open Python files? No, leave as is.</t>
+  </si>
+  <si>
+    <t>Two-Ball Collision Tracker Experiment 2019--deleted</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,10 +731,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1090,11 +1089,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1105,1037 +1104,1034 @@
     <col min="4" max="4" width="12.796875" customWidth="1"/>
     <col min="5" max="5" width="8.296875" customWidth="1"/>
     <col min="6" max="6" width="11.296875" customWidth="1"/>
-    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="23.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>56</v>
+      <c r="A42" t="s">
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" t="s">
+        <v>55</v>
+      </c>
+      <c r="E51" t="s">
+        <v>55</v>
+      </c>
+      <c r="G51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E52" t="s">
-        <v>56</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>